<commit_message>
Ajuste index y frame de estados
</commit_message>
<xml_diff>
--- a/public/templates/TemplateCargaDatosAcademusoft.xlsx
+++ b/public/templates/TemplateCargaDatosAcademusoft.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bitnami\wappstack-5.6.26-1\apache2\htdocs\Eva360\app\Uniajc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7815" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7815" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="UNIDAD" sheetId="3" r:id="rId1"/>
@@ -20,7 +15,7 @@
     <sheet name="DOCENTEUNIDAD" sheetId="5" r:id="rId6"/>
     <sheet name="DOCENTEGRUPO" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -140,18 +135,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>AAAA</t>
-  </si>
-  <si>
-    <t>BBBB</t>
-  </si>
-  <si>
-    <t>CCCC</t>
-  </si>
-  <si>
-    <t>DDDD</t>
-  </si>
-  <si>
     <t>HHH</t>
   </si>
   <si>
@@ -261,14 +244,34 @@
   </si>
   <si>
     <t>Robinson</t>
+  </si>
+  <si>
+    <t>BOLAÑOS</t>
+  </si>
+  <si>
+    <t>TAZ</t>
+  </si>
+  <si>
+    <t>CARLOS</t>
+  </si>
+  <si>
+    <t>ANDRES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -296,12 +299,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,7 +366,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -397,7 +401,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -574,7 +578,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -712,10 +716,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -723,10 +727,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -734,10 +738,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -745,10 +749,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -756,10 +760,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -801,7 +805,7 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>11</v>
@@ -896,7 +900,7 @@
         <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1049,7 +1053,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,36 +1106,36 @@
         <v>2222</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3333</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
@@ -1142,16 +1146,16 @@
         <v>4444</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>35</v>
@@ -1162,10 +1166,10 @@
         <v>5555</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -1176,10 +1180,10 @@
         <v>6666</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
@@ -1190,10 +1194,10 @@
         <v>7777</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
         <v>34</v>
@@ -1204,10 +1208,10 @@
         <v>8888</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
         <v>34</v>
@@ -1218,10 +1222,10 @@
         <v>9999</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
@@ -1232,10 +1236,10 @@
         <v>11111</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
         <v>34</v>
@@ -1246,10 +1250,10 @@
         <v>22222</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F12" t="s">
         <v>34</v>
@@ -1260,10 +1264,10 @@
         <v>33333</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
@@ -1274,10 +1278,10 @@
         <v>44444</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
         <v>34</v>
@@ -1288,10 +1292,10 @@
         <v>55555</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s">
         <v>34</v>

</xml_diff>